<commit_message>
Update a_psat templates, predict banners, data excel files
</commit_message>
<xml_diff>
--- a/a_psat/data/problem_update.xlsx
+++ b/a_psat/data/problem_update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483771AC-0C2F-4EC7-93DF-E0194078770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503EE2E4-0E8C-4719-8EE5-87EF1CDBA3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" xr2:uid="{B9E10960-7E98-404D-98CA-6EA27F27281D}"/>
   </bookViews>
@@ -2334,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B098CC65-4AD9-42F8-BC67-C5A258EBA4D4}">
   <dimension ref="A1:H426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="D409" sqref="D409"/>
+    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
+      <selection activeCell="A417" sqref="A417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>